<commit_message>
Changed Check Date and Service date for N70
</commit_message>
<xml_diff>
--- a/afa-invoice-report-validator/src/test/resources/input/Input.xlsx
+++ b/afa-invoice-report-validator/src/test/resources/input/Input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4DD9B-45A3-4C22-8417-52602EC95E7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FDBD6-C567-4238-9127-360A72675DBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>SL NO</t>
   </si>
   <si>
     <t>Invoice No</t>
   </si>
+  <si>
+    <t>191480000297</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,12 +59,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -64,7 +89,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,8 +395,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>191550000307</v>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>